<commit_message>
revision plan dep proeycto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1344 - CCON, Alfredo Gutierrez _ MO/Planeación/Plan_de_proyecto.xlsx
+++ b/Proyectos/2015/11/P1344 - CCON, Alfredo Gutierrez _ MO/Planeación/Plan_de_proyecto.xlsx
@@ -31,6 +31,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="Complej." vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area_0" vbProcedure="false">'Plan Riesgos'!$A$1:$F$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -592,7 +593,7 @@
     <t>Frecuencia de monitoreo</t>
   </si>
   <si>
-    <t>Falla de conexión remota con Ammyy Admin En caso de fallar la conexión remota con Ammy Admin por no instalación o problemas de equipo</t>
+    <t>En caso de fallar la conexión remota con Ammy Admin por no instalación o problemas de equipo afecta la comunicación en cliente soporte</t>
   </si>
   <si>
     <t>TeamViwer, Show myPC</t>
@@ -610,7 +611,7 @@
     <t>Semanal</t>
   </si>
   <si>
-    <t>En caso de presentar problemas de instalación y configuración por problemas de compatibilidad</t>
+    <t>En caso de presentar problemas de instalación y configuración por problemas de compatibilidad puede afectar la entrega del servicio e incluso cancelarlo</t>
   </si>
   <si>
     <t>Validar los requerimientos minimos del equipo</t>
@@ -622,7 +623,7 @@
     <t>Ocurrido</t>
   </si>
   <si>
-    <t>Falla de descarga de programa ocasionada por una conexión a internet pobre o limitada</t>
+    <t>Falla de descarga de programa ocasionada por una conexión a internet pobre o limitada aumenta el tiempo de instalación estimado en la etapa de implementación</t>
   </si>
   <si>
     <t>Validar que la descarga se halla realizado</t>
@@ -631,7 +632,7 @@
     <t>Reagenda la cita</t>
   </si>
   <si>
-    <t>Falla electrica por problemas variables que afecta el uso de dispositivos</t>
+    <t>Falla electrica por problemas variables que afecta el uso de dispositivos </t>
   </si>
   <si>
     <t>Home work</t>
@@ -658,7 +659,7 @@
     <t>MA</t>
   </si>
   <si>
-    <t>No obtener carta de aceptación por un cliente que no contesta mensajes</t>
+    <t>No obtener carta de aceptación por un cliente que no contesta mensajes afecta la etapa cierre de proyecto</t>
   </si>
   <si>
     <t>Enviar factura hasta obtener carta de aceptación</t>
@@ -1186,7 +1187,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1219,16 +1220,13 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="150">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1248,7 +1246,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1256,7 +1258,43 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1264,55 +1302,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1336,27 +1334,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1364,39 +1362,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1464,11 +1462,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1564,7 +1562,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1825,15 +1823,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -4607,6 +4604,27 @@
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
       <c r="E17" s="40"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
@@ -9333,8 +9351,8 @@
   </sheetPr>
   <dimension ref="A1:JA43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9445,7 +9463,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="82" t="n">
         <v>1</v>
       </c>
@@ -9481,7 +9499,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="82" t="n">
         <v>2</v>
       </c>
@@ -9517,7 +9535,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="82" t="n">
         <v>3</v>
       </c>
@@ -9553,7 +9571,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="82" t="n">
         <v>4</v>
       </c>
@@ -9662,7 +9680,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="101" t="n">
         <v>6</v>
       </c>

</xml_diff>